<commit_message>
Add description and color for diagrams
</commit_message>
<xml_diff>
--- a/docs/3_CAND_Modele_Journal_2024.xlsx
+++ b/docs/3_CAND_Modele_Journal_2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\tests\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3066F58E-B117-4C55-9E64-C329B83F6D2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{473600CF-63D1-40F3-916C-3E0B0A04C7E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Journal!$A$5:$HI$5</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Journal!$B:$D,Journal!$1:$5</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Journal!$A$1:$D$89</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Journal!$A$1:$D$87</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="35">
   <si>
     <t>Insérer les lignes au-dessus de celle-ci !</t>
   </si>
@@ -166,6 +166,24 @@
   <si>
     <t>Confirmation que la première visite c'est bien passée.
 Proposition d'une téchnique de rédaction pour la documentation</t>
+  </si>
+  <si>
+    <t>Correction du diagramme séquence système</t>
+  </si>
+  <si>
+    <t>Diagramme de classe</t>
+  </si>
+  <si>
+    <t>C'étais une très bonne journée et j'ai appris beaucoup de choses par rapport à la suite du projet. J'ai eus du mal à commencer la journée car j'étais un peu stressé de rencontrer les experts.</t>
+  </si>
+  <si>
+    <t>Diagrammes d'activités</t>
+  </si>
+  <si>
+    <t>Diagrammes de séquence d'interaction</t>
+  </si>
+  <si>
+    <t>Planification des tests fonctionnels</t>
   </si>
 </sst>
 </file>
@@ -679,7 +697,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -688,265 +706,240 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="22" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="22" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="22">
     <dxf>
       <font>
         <strike val="0"/>
@@ -1557,12 +1550,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H90"/>
+  <dimension ref="A1:H88"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft"/>
       <selection activeCell="D5" sqref="A5:XFD5"/>
-      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
+      <selection pane="bottomLeft" activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1575,918 +1568,916 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
     </row>
     <row r="2" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="31">
+      <c r="B2" s="59"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="21">
         <v>148477</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="14"/>
-      <c r="H3" s="15"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="8"/>
     </row>
     <row r="4" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="43"/>
-      <c r="D4" s="44" t="s">
+      <c r="C4" s="55"/>
+      <c r="D4" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="F4" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="11"/>
-      <c r="H4" s="17"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="10"/>
     </row>
     <row r="5" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="45"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="46" t="s">
+      <c r="A5" s="62"/>
+      <c r="B5" s="56"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="18" t="s">
+      <c r="F5" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G5" s="9"/>
-      <c r="H5" s="19"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="12"/>
     </row>
     <row r="6" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="47">
+      <c r="A6" s="38">
         <v>45433</v>
       </c>
-      <c r="B6" s="52" t="s">
+      <c r="B6" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="52"/>
-      <c r="D6" s="53">
+      <c r="C6" s="58"/>
+      <c r="D6" s="32">
         <v>1.5</v>
       </c>
-      <c r="F6" s="20" t="s">
+      <c r="F6" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="10"/>
-      <c r="H6" s="21"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="14"/>
     </row>
     <row r="7" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="55"/>
-      <c r="B7" s="32" t="s">
+      <c r="A7" s="39"/>
+      <c r="B7" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="32"/>
-      <c r="D7" s="54">
+      <c r="C7" s="51"/>
+      <c r="D7" s="33">
         <v>1</v>
       </c>
-      <c r="F7" s="22" t="s">
+      <c r="F7" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="23"/>
-      <c r="H7" s="24"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="17"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="55"/>
-      <c r="B8" s="27" t="s">
+      <c r="A8" s="39"/>
+      <c r="B8" s="52" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="27"/>
-      <c r="D8" s="51">
+      <c r="C8" s="52"/>
+      <c r="D8" s="31">
         <v>1</v>
       </c>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
     </row>
     <row r="9" spans="1:8" ht="56.25" x14ac:dyDescent="0.2">
-      <c r="A9" s="55"/>
-      <c r="B9" s="28" t="s">
+      <c r="A9" s="39"/>
+      <c r="B9" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="29" t="s">
+      <c r="C9" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="51">
+      <c r="D9" s="31">
         <v>0.5</v>
       </c>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="55"/>
-      <c r="B10" s="26"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="51">
+      <c r="A10" s="39"/>
+      <c r="B10" s="44"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="31">
         <v>1.5</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="55"/>
-      <c r="B11" s="26" t="s">
+      <c r="A11" s="39"/>
+      <c r="B11" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="26"/>
-      <c r="D11" s="51">
+      <c r="C11" s="44"/>
+      <c r="D11" s="31">
         <v>0.5</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="55"/>
-      <c r="B12" s="33" t="s">
+      <c r="A12" s="39"/>
+      <c r="B12" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="34" t="s">
+      <c r="C12" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="51">
+      <c r="D12" s="31">
         <v>1.5</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="55"/>
-      <c r="B13" s="35" t="s">
+      <c r="A13" s="39"/>
+      <c r="B13" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="36" t="s">
+      <c r="C13" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="51">
+      <c r="D13" s="31">
         <f>SUM(D6:D12)</f>
         <v>7.5</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="48"/>
-      <c r="B14" s="57" t="s">
+      <c r="A14" s="40"/>
+      <c r="B14" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="57"/>
-      <c r="D14" s="58"/>
+      <c r="C14" s="45"/>
+      <c r="D14" s="46"/>
     </row>
     <row r="15" spans="1:8" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A15" s="47">
+      <c r="A15" s="38">
         <v>45434</v>
       </c>
-      <c r="B15" s="59" t="s">
+      <c r="B15" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="60" t="s">
+      <c r="C15" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="61">
+      <c r="D15" s="37">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="55"/>
-      <c r="B16" s="37" t="s">
+      <c r="A16" s="39"/>
+      <c r="B16" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="37"/>
-      <c r="D16" s="51">
+      <c r="C16" s="41"/>
+      <c r="D16" s="31">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="55"/>
-      <c r="B17" s="30" t="s">
+      <c r="A17" s="39"/>
+      <c r="B17" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="30"/>
-      <c r="D17" s="51">
+      <c r="C17" s="48"/>
+      <c r="D17" s="31">
         <v>0.5</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="67.5" x14ac:dyDescent="0.2">
-      <c r="A18" s="55"/>
-      <c r="B18" s="28" t="s">
+      <c r="A18" s="39"/>
+      <c r="B18" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="38" t="s">
+      <c r="C18" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="51">
+      <c r="D18" s="31">
         <v>0.5</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.2">
-      <c r="A19" s="55"/>
-      <c r="B19" s="39" t="s">
+      <c r="A19" s="39"/>
+      <c r="B19" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="38" t="s">
+      <c r="C19" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="D19" s="51">
+      <c r="D19" s="31">
         <v>0.5</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="55"/>
-      <c r="B20" s="30"/>
-      <c r="C20" s="30"/>
-      <c r="D20" s="51"/>
+      <c r="A20" s="39"/>
+      <c r="B20" s="44" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="44"/>
+      <c r="D20" s="31">
+        <v>1</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="55"/>
-      <c r="B21" s="63"/>
-      <c r="C21" s="64"/>
-      <c r="D21" s="51"/>
+      <c r="A21" s="39"/>
+      <c r="B21" s="42" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="43"/>
+      <c r="D21" s="31">
+        <v>3.5</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="55"/>
-      <c r="B22" s="30"/>
-      <c r="C22" s="30"/>
-      <c r="D22" s="51"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="55"/>
-      <c r="B23" s="30"/>
-      <c r="C23" s="30"/>
-      <c r="D23" s="51"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="55"/>
-      <c r="B24" s="35" t="s">
+      <c r="A22" s="39"/>
+      <c r="B22" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="C24" s="36" t="s">
+      <c r="C22" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="D24" s="51">
-        <f>SUM(D15:D23)</f>
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="48"/>
-      <c r="B25" s="57"/>
-      <c r="C25" s="57"/>
-      <c r="D25" s="58"/>
-    </row>
-    <row r="26" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="47">
+      <c r="D22" s="31">
+        <f>SUM(D15:D21)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="40"/>
+      <c r="B23" s="45" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="45"/>
+      <c r="D23" s="46"/>
+    </row>
+    <row r="24" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="38">
         <v>45435</v>
       </c>
-      <c r="B26" s="62"/>
-      <c r="C26" s="62"/>
-      <c r="D26" s="61"/>
+      <c r="B24" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" s="41"/>
+      <c r="D24" s="37"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="39"/>
+      <c r="B25" s="42" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" s="43"/>
+      <c r="D25" s="31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="39"/>
+      <c r="B26" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" s="44"/>
+      <c r="D26" s="31">
+        <v>2.5</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="55"/>
-      <c r="B27" s="30"/>
-      <c r="C27" s="30"/>
-      <c r="D27" s="51"/>
+      <c r="A27" s="39"/>
+      <c r="B27" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27" s="44"/>
+      <c r="D27" s="31">
+        <v>2</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="55"/>
-      <c r="B28" s="30"/>
-      <c r="C28" s="30"/>
-      <c r="D28" s="51"/>
+      <c r="A28" s="39"/>
+      <c r="B28" s="44" t="s">
+        <v>34</v>
+      </c>
+      <c r="C28" s="44"/>
+      <c r="D28" s="31"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="55"/>
-      <c r="B29" s="30"/>
-      <c r="C29" s="30"/>
-      <c r="D29" s="51"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="55"/>
-      <c r="B30" s="30"/>
-      <c r="C30" s="30"/>
-      <c r="D30" s="51"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="55"/>
-      <c r="B31" s="35" t="s">
+      <c r="A29" s="39"/>
+      <c r="B29" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="C31" s="36" t="s">
+      <c r="C29" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="D31" s="51">
-        <f>SUM(D26:D30)</f>
+      <c r="D29" s="31">
+        <f>SUM(D24:D28)</f>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="40"/>
+      <c r="B30" s="45"/>
+      <c r="C30" s="45"/>
+      <c r="D30" s="46"/>
+    </row>
+    <row r="31" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="38">
+        <v>45436</v>
+      </c>
+      <c r="B31" s="47"/>
+      <c r="C31" s="47"/>
+      <c r="D31" s="37"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="39"/>
+      <c r="B32" s="48"/>
+      <c r="C32" s="48"/>
+      <c r="D32" s="31"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="39"/>
+      <c r="B33" s="48"/>
+      <c r="C33" s="48"/>
+      <c r="D33" s="31"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="39"/>
+      <c r="B34" s="48"/>
+      <c r="C34" s="48"/>
+      <c r="D34" s="31"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="39"/>
+      <c r="B35" s="48"/>
+      <c r="C35" s="48"/>
+      <c r="D35" s="31"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="39"/>
+      <c r="B36" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36" s="31">
+        <f>SUM(D31:D35)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="48"/>
-      <c r="B32" s="57"/>
-      <c r="C32" s="57"/>
-      <c r="D32" s="58"/>
-    </row>
-    <row r="33" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="47">
-        <v>45436</v>
-      </c>
-      <c r="B33" s="62"/>
-      <c r="C33" s="62"/>
-      <c r="D33" s="61"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="55"/>
-      <c r="B34" s="30"/>
-      <c r="C34" s="30"/>
-      <c r="D34" s="51"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="55"/>
-      <c r="B35" s="30"/>
-      <c r="C35" s="30"/>
-      <c r="D35" s="51"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="55"/>
-      <c r="B36" s="30"/>
-      <c r="C36" s="30"/>
-      <c r="D36" s="51"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="55"/>
-      <c r="B37" s="30"/>
-      <c r="C37" s="30"/>
-      <c r="D37" s="51"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="55"/>
-      <c r="B38" s="35" t="s">
+    <row r="37" spans="1:4" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="40"/>
+      <c r="B37" s="45"/>
+      <c r="C37" s="45"/>
+      <c r="D37" s="46"/>
+    </row>
+    <row r="38" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="38">
+        <v>45437</v>
+      </c>
+      <c r="B38" s="47"/>
+      <c r="C38" s="47"/>
+      <c r="D38" s="37"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="39"/>
+      <c r="B39" s="48"/>
+      <c r="C39" s="48"/>
+      <c r="D39" s="31"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="39"/>
+      <c r="B40" s="48"/>
+      <c r="C40" s="48"/>
+      <c r="D40" s="31"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="39"/>
+      <c r="B41" s="48"/>
+      <c r="C41" s="48"/>
+      <c r="D41" s="31"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="39"/>
+      <c r="B42" s="48"/>
+      <c r="C42" s="48"/>
+      <c r="D42" s="31"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="39"/>
+      <c r="B43" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="C38" s="36" t="s">
+      <c r="C43" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="D38" s="51">
-        <f>SUM(D33:D37)</f>
+      <c r="D43" s="31">
+        <f>SUM(D38:D42)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="48"/>
-      <c r="B39" s="57"/>
-      <c r="C39" s="57"/>
-      <c r="D39" s="58"/>
-    </row>
-    <row r="40" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="47">
-        <v>45437</v>
-      </c>
-      <c r="B40" s="62"/>
-      <c r="C40" s="62"/>
-      <c r="D40" s="61"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="55"/>
-      <c r="B41" s="30"/>
-      <c r="C41" s="30"/>
-      <c r="D41" s="51"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="55"/>
-      <c r="B42" s="30"/>
-      <c r="C42" s="30"/>
-      <c r="D42" s="51"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="55"/>
-      <c r="B43" s="30"/>
-      <c r="C43" s="30"/>
-      <c r="D43" s="51"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="55"/>
-      <c r="B44" s="30"/>
-      <c r="C44" s="30"/>
-      <c r="D44" s="51"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="55"/>
-      <c r="B45" s="35" t="s">
+    <row r="44" spans="1:4" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="40"/>
+      <c r="B44" s="45"/>
+      <c r="C44" s="45"/>
+      <c r="D44" s="46"/>
+    </row>
+    <row r="45" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="38"/>
+      <c r="B45" s="47"/>
+      <c r="C45" s="47"/>
+      <c r="D45" s="37"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="39"/>
+      <c r="B46" s="48"/>
+      <c r="C46" s="48"/>
+      <c r="D46" s="31"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="39"/>
+      <c r="B47" s="48"/>
+      <c r="C47" s="48"/>
+      <c r="D47" s="31"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="39"/>
+      <c r="B48" s="48"/>
+      <c r="C48" s="48"/>
+      <c r="D48" s="31"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="39"/>
+      <c r="B49" s="48"/>
+      <c r="C49" s="48"/>
+      <c r="D49" s="31"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="39"/>
+      <c r="B50" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="C45" s="36" t="s">
+      <c r="C50" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="D45" s="51">
-        <f>SUM(D40:D44)</f>
+      <c r="D50" s="31">
+        <f>SUM(D45:D49)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="48"/>
-      <c r="B46" s="57"/>
-      <c r="C46" s="57"/>
-      <c r="D46" s="58"/>
-    </row>
-    <row r="47" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="47"/>
-      <c r="B47" s="62"/>
-      <c r="C47" s="62"/>
-      <c r="D47" s="61"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" s="55"/>
-      <c r="B48" s="30"/>
-      <c r="C48" s="30"/>
-      <c r="D48" s="51"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="55"/>
-      <c r="B49" s="30"/>
-      <c r="C49" s="30"/>
-      <c r="D49" s="51"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" s="55"/>
-      <c r="B50" s="30"/>
-      <c r="C50" s="30"/>
-      <c r="D50" s="51"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" s="55"/>
-      <c r="B51" s="30"/>
-      <c r="C51" s="30"/>
-      <c r="D51" s="51"/>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" s="55"/>
-      <c r="B52" s="35" t="s">
+    <row r="51" spans="1:4" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="40"/>
+      <c r="B51" s="45"/>
+      <c r="C51" s="45"/>
+      <c r="D51" s="46"/>
+    </row>
+    <row r="52" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="38"/>
+      <c r="B52" s="47"/>
+      <c r="C52" s="47"/>
+      <c r="D52" s="37"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="39"/>
+      <c r="B53" s="48"/>
+      <c r="C53" s="48"/>
+      <c r="D53" s="31"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="39"/>
+      <c r="B54" s="48"/>
+      <c r="C54" s="48"/>
+      <c r="D54" s="31"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" s="39"/>
+      <c r="B55" s="48"/>
+      <c r="C55" s="48"/>
+      <c r="D55" s="31"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" s="39"/>
+      <c r="B56" s="48"/>
+      <c r="C56" s="48"/>
+      <c r="D56" s="31"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" s="39"/>
+      <c r="B57" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="C52" s="36" t="s">
+      <c r="C57" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="D52" s="51">
-        <f>SUM(D47:D51)</f>
+      <c r="D57" s="31">
+        <f>SUM(D52:D56)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="48"/>
-      <c r="B53" s="57"/>
-      <c r="C53" s="57"/>
-      <c r="D53" s="58"/>
-    </row>
-    <row r="54" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="47"/>
-      <c r="B54" s="62"/>
-      <c r="C54" s="62"/>
-      <c r="D54" s="61"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" s="55"/>
-      <c r="B55" s="30"/>
-      <c r="C55" s="30"/>
-      <c r="D55" s="51"/>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" s="55"/>
-      <c r="B56" s="30"/>
-      <c r="C56" s="30"/>
-      <c r="D56" s="51"/>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" s="55"/>
-      <c r="B57" s="30"/>
-      <c r="C57" s="30"/>
-      <c r="D57" s="51"/>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" s="55"/>
-      <c r="B58" s="30"/>
-      <c r="C58" s="30"/>
-      <c r="D58" s="51"/>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" s="55"/>
-      <c r="B59" s="35" t="s">
+    <row r="58" spans="1:4" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="40"/>
+      <c r="B58" s="45"/>
+      <c r="C58" s="45"/>
+      <c r="D58" s="46"/>
+    </row>
+    <row r="59" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="38"/>
+      <c r="B59" s="47"/>
+      <c r="C59" s="47"/>
+      <c r="D59" s="37"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" s="39"/>
+      <c r="B60" s="48"/>
+      <c r="C60" s="48"/>
+      <c r="D60" s="31"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" s="39"/>
+      <c r="B61" s="48"/>
+      <c r="C61" s="48"/>
+      <c r="D61" s="31"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" s="39"/>
+      <c r="B62" s="48"/>
+      <c r="C62" s="48"/>
+      <c r="D62" s="31"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" s="39"/>
+      <c r="B63" s="48"/>
+      <c r="C63" s="48"/>
+      <c r="D63" s="31"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" s="39"/>
+      <c r="B64" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="C59" s="36" t="s">
+      <c r="C64" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="D59" s="51">
-        <f>SUM(D54:D58)</f>
+      <c r="D64" s="31">
+        <f>SUM(D59:D63)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="48"/>
-      <c r="B60" s="57"/>
-      <c r="C60" s="57"/>
-      <c r="D60" s="58"/>
-    </row>
-    <row r="61" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="47"/>
-      <c r="B61" s="62"/>
-      <c r="C61" s="62"/>
-      <c r="D61" s="61"/>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" s="55"/>
-      <c r="B62" s="30"/>
-      <c r="C62" s="30"/>
-      <c r="D62" s="51"/>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" s="55"/>
-      <c r="B63" s="30"/>
-      <c r="C63" s="30"/>
-      <c r="D63" s="51"/>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" s="55"/>
-      <c r="B64" s="30"/>
-      <c r="C64" s="30"/>
-      <c r="D64" s="51"/>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" s="55"/>
-      <c r="B65" s="30"/>
-      <c r="C65" s="30"/>
-      <c r="D65" s="51"/>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" s="55"/>
-      <c r="B66" s="35" t="s">
+    <row r="65" spans="1:4" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="40"/>
+      <c r="B65" s="45"/>
+      <c r="C65" s="45"/>
+      <c r="D65" s="46"/>
+    </row>
+    <row r="66" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="38"/>
+      <c r="B66" s="47"/>
+      <c r="C66" s="47"/>
+      <c r="D66" s="37"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" s="39"/>
+      <c r="B67" s="48"/>
+      <c r="C67" s="48"/>
+      <c r="D67" s="31"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" s="39"/>
+      <c r="B68" s="48"/>
+      <c r="C68" s="48"/>
+      <c r="D68" s="31"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" s="39"/>
+      <c r="B69" s="48"/>
+      <c r="C69" s="48"/>
+      <c r="D69" s="31"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" s="39"/>
+      <c r="B70" s="48"/>
+      <c r="C70" s="48"/>
+      <c r="D70" s="31"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" s="39"/>
+      <c r="B71" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="C66" s="36" t="s">
+      <c r="C71" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="D66" s="51">
-        <f>SUM(D61:D65)</f>
+      <c r="D71" s="31">
+        <f>SUM(D66:D70)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="48"/>
-      <c r="B67" s="57"/>
-      <c r="C67" s="57"/>
-      <c r="D67" s="58"/>
-    </row>
-    <row r="68" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="47"/>
-      <c r="B68" s="62"/>
-      <c r="C68" s="62"/>
-      <c r="D68" s="61"/>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69" s="55"/>
-      <c r="B69" s="30"/>
-      <c r="C69" s="30"/>
-      <c r="D69" s="51"/>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" s="55"/>
-      <c r="B70" s="30"/>
-      <c r="C70" s="30"/>
-      <c r="D70" s="51"/>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" s="55"/>
-      <c r="B71" s="30"/>
-      <c r="C71" s="30"/>
-      <c r="D71" s="51"/>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" s="55"/>
-      <c r="B72" s="30"/>
-      <c r="C72" s="30"/>
-      <c r="D72" s="51"/>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" s="55"/>
-      <c r="B73" s="35" t="s">
+    <row r="72" spans="1:4" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="40"/>
+      <c r="B72" s="45"/>
+      <c r="C72" s="45"/>
+      <c r="D72" s="46"/>
+    </row>
+    <row r="73" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="38"/>
+      <c r="B73" s="47"/>
+      <c r="C73" s="47"/>
+      <c r="D73" s="37"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74" s="39"/>
+      <c r="B74" s="48"/>
+      <c r="C74" s="48"/>
+      <c r="D74" s="31"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75" s="39"/>
+      <c r="B75" s="48"/>
+      <c r="C75" s="48"/>
+      <c r="D75" s="31"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76" s="39"/>
+      <c r="B76" s="48"/>
+      <c r="C76" s="48"/>
+      <c r="D76" s="31"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77" s="39"/>
+      <c r="B77" s="48"/>
+      <c r="C77" s="48"/>
+      <c r="D77" s="31"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78" s="39"/>
+      <c r="B78" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="C73" s="36" t="s">
+      <c r="C78" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="D73" s="51">
-        <f>SUM(D68:D72)</f>
+      <c r="D78" s="31">
+        <f>SUM(D73:D77)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="48"/>
-      <c r="B74" s="57"/>
-      <c r="C74" s="57"/>
-      <c r="D74" s="58"/>
-    </row>
-    <row r="75" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="47"/>
-      <c r="B75" s="62"/>
-      <c r="C75" s="62"/>
-      <c r="D75" s="61"/>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A76" s="55"/>
-      <c r="B76" s="30"/>
-      <c r="C76" s="30"/>
-      <c r="D76" s="51"/>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A77" s="55"/>
-      <c r="B77" s="30"/>
-      <c r="C77" s="30"/>
-      <c r="D77" s="51"/>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A78" s="55"/>
-      <c r="B78" s="30"/>
-      <c r="C78" s="30"/>
-      <c r="D78" s="51"/>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79" s="55"/>
-      <c r="B79" s="30"/>
-      <c r="C79" s="30"/>
-      <c r="D79" s="51"/>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80" s="55"/>
-      <c r="B80" s="35" t="s">
+    <row r="79" spans="1:4" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="40"/>
+      <c r="B79" s="45"/>
+      <c r="C79" s="45"/>
+      <c r="D79" s="46"/>
+    </row>
+    <row r="80" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="38"/>
+      <c r="B80" s="47"/>
+      <c r="C80" s="47"/>
+      <c r="D80" s="37"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A81" s="39"/>
+      <c r="B81" s="48"/>
+      <c r="C81" s="48"/>
+      <c r="D81" s="31"/>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A82" s="39"/>
+      <c r="B82" s="48"/>
+      <c r="C82" s="48"/>
+      <c r="D82" s="31"/>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83" s="39"/>
+      <c r="B83" s="48"/>
+      <c r="C83" s="48"/>
+      <c r="D83" s="31"/>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A84" s="39"/>
+      <c r="B84" s="48"/>
+      <c r="C84" s="48"/>
+      <c r="D84" s="31"/>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A85" s="39"/>
+      <c r="B85" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="C80" s="36" t="s">
+      <c r="C85" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="D80" s="51">
-        <f>SUM(D75:D79)</f>
+      <c r="D85" s="31">
+        <f>SUM(D80:D84)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="48"/>
-      <c r="B81" s="57"/>
-      <c r="C81" s="57"/>
-      <c r="D81" s="58"/>
-    </row>
-    <row r="82" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="47"/>
-      <c r="B82" s="62"/>
-      <c r="C82" s="62"/>
-      <c r="D82" s="61"/>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A83" s="55"/>
-      <c r="B83" s="30"/>
-      <c r="C83" s="30"/>
-      <c r="D83" s="51"/>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A84" s="55"/>
-      <c r="B84" s="30"/>
-      <c r="C84" s="30"/>
-      <c r="D84" s="51"/>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A85" s="55"/>
-      <c r="B85" s="30"/>
-      <c r="C85" s="30"/>
-      <c r="D85" s="51"/>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A86" s="55"/>
-      <c r="B86" s="30"/>
-      <c r="C86" s="30"/>
-      <c r="D86" s="51"/>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A87" s="55"/>
-      <c r="B87" s="35" t="s">
-        <v>6</v>
-      </c>
-      <c r="C87" s="36" t="s">
-        <v>5</v>
-      </c>
-      <c r="D87" s="51">
-        <f>SUM(D82:D86)</f>
+    <row r="86" spans="1:4" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="40"/>
+      <c r="B86" s="49"/>
+      <c r="C86" s="49"/>
+      <c r="D86" s="50"/>
+    </row>
+    <row r="87" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="34"/>
+      <c r="B87" s="2"/>
+      <c r="C87" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D87" s="28">
+        <f>D13+D22+D29+D36+D43+D50+D57+D64+D71+D78+D85</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A88" s="63" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="48"/>
-      <c r="B88" s="49"/>
-      <c r="C88" s="49"/>
-      <c r="D88" s="50"/>
-    </row>
-    <row r="89" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="56"/>
-      <c r="B89" s="2"/>
-      <c r="C89" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="D89" s="40">
-        <f>D13+D24+D31+D38+D45+D52+D59+D66+D73+D80+D87</f>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A90" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B90" s="3"/>
-      <c r="C90" s="3"/>
-      <c r="D90" s="3"/>
+      <c r="B88" s="63"/>
+      <c r="C88" s="63"/>
+      <c r="D88" s="63"/>
     </row>
   </sheetData>
-  <mergeCells count="83">
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="A26:A32"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="B60:D60"/>
-    <mergeCell ref="A61:A67"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B67:D67"/>
+  <mergeCells count="81">
+    <mergeCell ref="A88:D88"/>
+    <mergeCell ref="A15:A23"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="A31:A37"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="A38:A44"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="B4:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A52:A58"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
     <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="A82:A88"/>
-    <mergeCell ref="B82:C82"/>
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="B84:C84"/>
-    <mergeCell ref="B85:C85"/>
-    <mergeCell ref="B86:C86"/>
-    <mergeCell ref="B88:D88"/>
-    <mergeCell ref="A75:A81"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="B78:C78"/>
-    <mergeCell ref="B79:C79"/>
-    <mergeCell ref="B81:D81"/>
-    <mergeCell ref="B46:D46"/>
-    <mergeCell ref="A68:A74"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B74:D74"/>
-    <mergeCell ref="A47:A53"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B53:D53"/>
-    <mergeCell ref="A54:A60"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="A6:A14"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B11:C11"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="B4:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A90:D90"/>
-    <mergeCell ref="A15:A25"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="A33:A39"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="A40:A46"/>
+    <mergeCell ref="A45:A51"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="A73:A79"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="B79:D79"/>
+    <mergeCell ref="A59:A65"/>
+    <mergeCell ref="A66:A72"/>
+    <mergeCell ref="B65:D65"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B72:D72"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="A80:A86"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="B82:C82"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="B84:C84"/>
+    <mergeCell ref="B86:D86"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B58:D58"/>
+    <mergeCell ref="A24:A30"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B26:C26"/>
   </mergeCells>
-  <conditionalFormatting sqref="D6:D13">
-    <cfRule type="containsText" dxfId="23" priority="23" operator="containsText" text="Terminé">
+  <conditionalFormatting sqref="D6:D13 D15:D22">
+    <cfRule type="containsText" dxfId="21" priority="23" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",D6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="24" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="20" priority="24" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",D6)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D15:D24">
-    <cfRule type="containsText" dxfId="21" priority="21" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",D15)))</formula>
+  <conditionalFormatting sqref="D24:D29">
+    <cfRule type="containsText" dxfId="19" priority="3" operator="containsText" text="Terminé">
+      <formula>NOT(ISERROR(SEARCH("Terminé",D24)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="22" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",D15)))</formula>
+    <cfRule type="containsText" dxfId="18" priority="4" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",D24)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D26:D31">
-    <cfRule type="containsText" dxfId="19" priority="3" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",D26)))</formula>
+  <conditionalFormatting sqref="D31:D36">
+    <cfRule type="containsText" dxfId="17" priority="19" operator="containsText" text="Terminé">
+      <formula>NOT(ISERROR(SEARCH("Terminé",D31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="4" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",D26)))</formula>
+    <cfRule type="containsText" dxfId="16" priority="20" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",D31)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D33:D38">
-    <cfRule type="containsText" dxfId="17" priority="19" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",D33)))</formula>
+  <conditionalFormatting sqref="D38:D43">
+    <cfRule type="containsText" dxfId="15" priority="17" operator="containsText" text="Terminé">
+      <formula>NOT(ISERROR(SEARCH("Terminé",D38)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="20" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",D33)))</formula>
+    <cfRule type="containsText" dxfId="14" priority="18" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",D38)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D40:D45">
-    <cfRule type="containsText" dxfId="15" priority="17" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",D40)))</formula>
+  <conditionalFormatting sqref="D45:D50">
+    <cfRule type="containsText" dxfId="13" priority="9" operator="containsText" text="Terminé">
+      <formula>NOT(ISERROR(SEARCH("Terminé",D45)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="18" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",D40)))</formula>
+    <cfRule type="containsText" dxfId="12" priority="10" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",D45)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D47:D52">
-    <cfRule type="containsText" dxfId="13" priority="9" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",D47)))</formula>
+  <conditionalFormatting sqref="D52:D57">
+    <cfRule type="containsText" dxfId="11" priority="7" operator="containsText" text="Terminé">
+      <formula>NOT(ISERROR(SEARCH("Terminé",D52)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="10" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",D47)))</formula>
+    <cfRule type="containsText" dxfId="10" priority="8" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",D52)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D54:D59">
-    <cfRule type="containsText" dxfId="11" priority="7" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",D54)))</formula>
+  <conditionalFormatting sqref="D59:D64">
+    <cfRule type="containsText" dxfId="9" priority="5" operator="containsText" text="Terminé">
+      <formula>NOT(ISERROR(SEARCH("Terminé",D59)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="8" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",D54)))</formula>
+    <cfRule type="containsText" dxfId="8" priority="6" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",D59)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D61:D66">
-    <cfRule type="containsText" dxfId="9" priority="5" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",D61)))</formula>
+  <conditionalFormatting sqref="D66:D71">
+    <cfRule type="containsText" dxfId="7" priority="15" operator="containsText" text="Terminé">
+      <formula>NOT(ISERROR(SEARCH("Terminé",D66)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="6" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",D61)))</formula>
+    <cfRule type="containsText" dxfId="6" priority="16" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",D66)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D68:D73">
-    <cfRule type="containsText" dxfId="7" priority="15" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",D68)))</formula>
+  <conditionalFormatting sqref="D73:D78">
+    <cfRule type="containsText" dxfId="5" priority="13" operator="containsText" text="Terminé">
+      <formula>NOT(ISERROR(SEARCH("Terminé",D73)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="16" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",D68)))</formula>
+    <cfRule type="containsText" dxfId="4" priority="14" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",D73)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D75:D80">
-    <cfRule type="containsText" dxfId="5" priority="13" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",D75)))</formula>
+  <conditionalFormatting sqref="D80:D85">
+    <cfRule type="containsText" dxfId="3" priority="11" operator="containsText" text="Terminé">
+      <formula>NOT(ISERROR(SEARCH("Terminé",D80)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="14" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",D75)))</formula>
+    <cfRule type="containsText" dxfId="2" priority="12" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",D80)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D82:D87">
-    <cfRule type="containsText" dxfId="3" priority="11" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",D82)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="12" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",D82)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D89">
+  <conditionalFormatting sqref="D87">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",D89)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Terminé",D87)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",D89)))</formula>
+      <formula>NOT(ISERROR(SEARCH("En cours",D87)))</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions horizontalCentered="1"/>
@@ -2498,8 +2489,8 @@
     <oddFooter>&amp;L&amp;8&amp;F&amp;R&amp;8Page &amp;P/&amp;N</oddFooter>
   </headerFooter>
   <rowBreaks count="2" manualBreakCount="2">
-    <brk id="53" max="16383" man="1"/>
-    <brk id="89" max="3" man="1"/>
+    <brk id="51" max="16383" man="1"/>
+    <brk id="87" max="3" man="1"/>
   </rowBreaks>
   <legacyDrawingHF r:id="rId2"/>
 </worksheet>

</xml_diff>

<commit_message>
Add database + DB requests
</commit_message>
<xml_diff>
--- a/docs/3_CAND_Modele_Journal_2024.xlsx
+++ b/docs/3_CAND_Modele_Journal_2024.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr checkCompatibility="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/HOME/alikadev/code/TPI/RoadTrafficSimulator/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\tests\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A880B6F7-85B6-404D-B29E-691463002478}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{542307CD-9746-4377-AD67-D0C85B2AEDEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="14400" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-165" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal" sheetId="8" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Journal!$A$5:$HI$5</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">Journal!$B:$D,Journal!$1:$5</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Journal!$A$1:$D$84</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">Journal!$B:$D,Journal!$1:$5</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="39">
   <si>
     <t>Insérer les lignes au-dessus de celle-ci !</t>
   </si>
@@ -192,6 +192,12 @@
   </si>
   <si>
     <t>J'ai bien avencé sur la documentation aujourd'hui et la totalité des diagrammes sont corrigé et confirmer. Je suis un peu en retard sur l'implémentation mais une demi journée n'est pas dramatique!</t>
+  </si>
+  <si>
+    <t>Implémenter la DB</t>
+  </si>
+  <si>
+    <t>Préparer les requêtes de la DB</t>
   </si>
 </sst>
 </file>
@@ -705,7 +711,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -835,6 +841,26 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
@@ -843,28 +869,76 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -875,71 +949,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -955,84 +965,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1109,6 +1042,17 @@
       </font>
       <fill>
         <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
@@ -1131,6 +1075,17 @@
       </font>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
@@ -1143,6 +1098,61 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1516,54 +1526,54 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="180" zoomScaleNormal="130" zoomScaleSheetLayoutView="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="130" zoomScaleSheetLayoutView="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft"/>
       <selection activeCell="D5" sqref="A5:XFD5"/>
-      <selection pane="bottomLeft" activeCell="D35" sqref="D35"/>
+      <selection pane="bottomLeft" activeCell="B37" sqref="B37:C37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.5" style="1"/>
-    <col min="2" max="3" width="31.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.6640625" style="1" customWidth="1"/>
-    <col min="5" max="217" width="9.1640625" style="1" customWidth="1"/>
-    <col min="218" max="16384" width="11.5" style="1"/>
+    <col min="1" max="1" width="11.42578125" style="1"/>
+    <col min="2" max="3" width="31.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" style="1" customWidth="1"/>
+    <col min="5" max="217" width="9.140625" style="1" customWidth="1"/>
+    <col min="218" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="20" x14ac:dyDescent="0.2">
-      <c r="A1" s="52" t="s">
+    <row r="1" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A1" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-    </row>
-    <row r="2" spans="1:8" ht="19" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="58" t="s">
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+    </row>
+    <row r="2" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="58"/>
-      <c r="C2" s="59"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="54"/>
       <c r="D2" s="21">
         <v>148477</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F3" s="6" t="s">
         <v>10</v>
       </c>
       <c r="G3" s="7"/>
       <c r="H3" s="8"/>
     </row>
-    <row r="4" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="60" t="s">
+    <row r="4" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="53" t="s">
+      <c r="B4" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="54"/>
+      <c r="C4" s="49"/>
       <c r="D4" s="28" t="s">
         <v>4</v>
       </c>
@@ -1573,10 +1583,10 @@
       <c r="G4" s="5"/>
       <c r="H4" s="10"/>
     </row>
-    <row r="5" spans="1:8" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="61"/>
-      <c r="B5" s="55"/>
-      <c r="C5" s="56"/>
+    <row r="5" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="56"/>
+      <c r="B5" s="50"/>
+      <c r="C5" s="51"/>
       <c r="D5" s="29" t="s">
         <v>3</v>
       </c>
@@ -1586,14 +1596,14 @@
       <c r="G5" s="3"/>
       <c r="H5" s="12"/>
     </row>
-    <row r="6" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="42">
+    <row r="6" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="38">
         <v>45433</v>
       </c>
-      <c r="B6" s="57" t="s">
+      <c r="B6" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="57"/>
+      <c r="C6" s="52"/>
       <c r="D6" s="31">
         <v>1.5</v>
       </c>
@@ -1603,12 +1613,12 @@
       <c r="G6" s="4"/>
       <c r="H6" s="14"/>
     </row>
-    <row r="7" spans="1:8" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="43"/>
-      <c r="B7" s="47" t="s">
+    <row r="7" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="39"/>
+      <c r="B7" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="47"/>
+      <c r="C7" s="60"/>
       <c r="D7" s="32">
         <v>1</v>
       </c>
@@ -1618,18 +1628,18 @@
       <c r="G7" s="16"/>
       <c r="H7" s="17"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A8" s="43"/>
-      <c r="B8" s="48" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="39"/>
+      <c r="B8" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="48"/>
+      <c r="C8" s="61"/>
       <c r="D8" s="30">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="60" x14ac:dyDescent="0.15">
-      <c r="A9" s="43"/>
+    <row r="9" spans="1:8" ht="56.25" x14ac:dyDescent="0.2">
+      <c r="A9" s="39"/>
       <c r="B9" s="19" t="s">
         <v>27</v>
       </c>
@@ -1640,26 +1650,26 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A10" s="43"/>
-      <c r="B10" s="39"/>
-      <c r="C10" s="39"/>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="39"/>
+      <c r="B10" s="45"/>
+      <c r="C10" s="45"/>
       <c r="D10" s="30">
         <v>1.5</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A11" s="43"/>
-      <c r="B11" s="39" t="s">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="39"/>
+      <c r="B11" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="39"/>
+      <c r="C11" s="45"/>
       <c r="D11" s="30">
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A12" s="43"/>
+    <row r="12" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A12" s="39"/>
       <c r="B12" s="22" t="s">
         <v>21</v>
       </c>
@@ -1670,8 +1680,8 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A13" s="43"/>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="39"/>
       <c r="B13" s="24" t="s">
         <v>6</v>
       </c>
@@ -1683,16 +1693,16 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="44"/>
-      <c r="B14" s="37" t="s">
+    <row r="14" spans="1:8" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="40"/>
+      <c r="B14" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="37"/>
-      <c r="D14" s="38"/>
-    </row>
-    <row r="15" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A15" s="42">
+      <c r="C14" s="42"/>
+      <c r="D14" s="43"/>
+    </row>
+    <row r="15" spans="1:8" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A15" s="38">
         <v>45434</v>
       </c>
       <c r="B15" s="34" t="s">
@@ -1705,28 +1715,28 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="43"/>
-      <c r="B16" s="49" t="s">
+    <row r="16" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="39"/>
+      <c r="B16" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="49"/>
+      <c r="C16" s="57"/>
       <c r="D16" s="30">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A17" s="43"/>
-      <c r="B17" s="40" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="39"/>
+      <c r="B17" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="40"/>
+      <c r="C17" s="41"/>
       <c r="D17" s="30">
         <v>0.5</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="60" x14ac:dyDescent="0.15">
-      <c r="A18" s="43"/>
+    <row r="18" spans="1:4" ht="67.5" x14ac:dyDescent="0.2">
+      <c r="A18" s="39"/>
       <c r="B18" s="19" t="s">
         <v>14</v>
       </c>
@@ -1737,8 +1747,8 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="36" x14ac:dyDescent="0.15">
-      <c r="A19" s="43"/>
+    <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.2">
+      <c r="A19" s="39"/>
       <c r="B19" s="19" t="s">
         <v>27</v>
       </c>
@@ -1749,28 +1759,28 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A20" s="43"/>
-      <c r="B20" s="39" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="39"/>
+      <c r="B20" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="39"/>
+      <c r="C20" s="45"/>
       <c r="D20" s="30">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A21" s="43"/>
-      <c r="B21" s="50" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="39"/>
+      <c r="B21" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="51"/>
+      <c r="C21" s="59"/>
       <c r="D21" s="30">
         <v>3.5</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A22" s="43"/>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="39"/>
       <c r="B22" s="24" t="s">
         <v>6</v>
       </c>
@@ -1782,56 +1792,56 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="44"/>
-      <c r="B23" s="37" t="s">
+    <row r="23" spans="1:4" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="40"/>
+      <c r="B23" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="C23" s="37"/>
-      <c r="D23" s="38"/>
-    </row>
-    <row r="24" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="42">
+      <c r="C23" s="42"/>
+      <c r="D23" s="43"/>
+    </row>
+    <row r="24" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="38">
         <v>45435</v>
       </c>
-      <c r="B24" s="49" t="s">
+      <c r="B24" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="C24" s="49"/>
+      <c r="C24" s="57"/>
       <c r="D24" s="36"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A25" s="43"/>
-      <c r="B25" s="50" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="39"/>
+      <c r="B25" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="51"/>
+      <c r="C25" s="59"/>
       <c r="D25" s="30">
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A26" s="43"/>
-      <c r="B26" s="39" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="39"/>
+      <c r="B26" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="C26" s="39"/>
+      <c r="C26" s="45"/>
       <c r="D26" s="30">
         <v>2.5</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A27" s="43"/>
-      <c r="B27" s="39" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="39"/>
+      <c r="B27" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="C27" s="39"/>
+      <c r="C27" s="45"/>
       <c r="D27" s="30">
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A28" s="43"/>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="39"/>
       <c r="B28" s="24" t="s">
         <v>6</v>
       </c>
@@ -1843,26 +1853,26 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="44"/>
-      <c r="B29" s="37"/>
-      <c r="C29" s="37"/>
-      <c r="D29" s="38"/>
-    </row>
-    <row r="30" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="42">
+    <row r="29" spans="1:4" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="40"/>
+      <c r="B29" s="42"/>
+      <c r="C29" s="42"/>
+      <c r="D29" s="43"/>
+    </row>
+    <row r="30" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="38">
         <v>45436</v>
       </c>
-      <c r="B30" s="63" t="s">
+      <c r="B30" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="C30" s="63"/>
+      <c r="C30" s="44"/>
       <c r="D30" s="36">
         <v>4.5</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="60" x14ac:dyDescent="0.15">
-      <c r="A31" s="43"/>
+    <row r="31" spans="1:4" ht="56.25" x14ac:dyDescent="0.2">
+      <c r="A31" s="39"/>
       <c r="B31" s="19" t="s">
         <v>27</v>
       </c>
@@ -1873,18 +1883,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A32" s="43"/>
-      <c r="B32" s="39" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="39"/>
+      <c r="B32" s="45" t="s">
         <v>35</v>
       </c>
-      <c r="C32" s="39"/>
+      <c r="C32" s="45"/>
       <c r="D32" s="30">
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A33" s="43"/>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="39"/>
       <c r="B33" s="24" t="s">
         <v>6</v>
       </c>
@@ -1896,48 +1906,56 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="44"/>
-      <c r="B34" s="37" t="s">
+    <row r="34" spans="1:4" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="40"/>
+      <c r="B34" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="C34" s="37"/>
-      <c r="D34" s="38"/>
-    </row>
-    <row r="35" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="42">
+      <c r="C34" s="42"/>
+      <c r="D34" s="43"/>
+    </row>
+    <row r="35" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="38">
         <v>45439</v>
       </c>
-      <c r="B35" s="41"/>
-      <c r="C35" s="41"/>
-      <c r="D35" s="36"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A36" s="43"/>
-      <c r="B36" s="40"/>
-      <c r="C36" s="40"/>
-      <c r="D36" s="30"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A37" s="43"/>
-      <c r="B37" s="40"/>
-      <c r="C37" s="40"/>
+      <c r="B35" s="64" t="s">
+        <v>37</v>
+      </c>
+      <c r="C35" s="64"/>
+      <c r="D35" s="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="39"/>
+      <c r="B36" s="45" t="s">
+        <v>38</v>
+      </c>
+      <c r="C36" s="45"/>
+      <c r="D36" s="30">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="39"/>
+      <c r="B37" s="41"/>
+      <c r="C37" s="41"/>
       <c r="D37" s="30"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A38" s="43"/>
-      <c r="B38" s="40"/>
-      <c r="C38" s="40"/>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="39"/>
+      <c r="B38" s="41"/>
+      <c r="C38" s="41"/>
       <c r="D38" s="30"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A39" s="43"/>
-      <c r="B39" s="40"/>
-      <c r="C39" s="40"/>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="39"/>
+      <c r="B39" s="41"/>
+      <c r="C39" s="41"/>
       <c r="D39" s="30"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A40" s="43"/>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="39"/>
       <c r="B40" s="24" t="s">
         <v>6</v>
       </c>
@@ -1946,49 +1964,49 @@
       </c>
       <c r="D40" s="30">
         <f>SUM(D35:D39)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="44"/>
-      <c r="B41" s="37"/>
-      <c r="C41" s="37"/>
-      <c r="D41" s="38"/>
-    </row>
-    <row r="42" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="42">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="40"/>
+      <c r="B41" s="42"/>
+      <c r="C41" s="42"/>
+      <c r="D41" s="43"/>
+    </row>
+    <row r="42" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="38">
         <v>45440</v>
       </c>
-      <c r="B42" s="41"/>
-      <c r="C42" s="41"/>
+      <c r="B42" s="46"/>
+      <c r="C42" s="46"/>
       <c r="D42" s="36"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A43" s="43"/>
-      <c r="B43" s="40"/>
-      <c r="C43" s="40"/>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="39"/>
+      <c r="B43" s="41"/>
+      <c r="C43" s="41"/>
       <c r="D43" s="30"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A44" s="43"/>
-      <c r="B44" s="40"/>
-      <c r="C44" s="40"/>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="39"/>
+      <c r="B44" s="41"/>
+      <c r="C44" s="41"/>
       <c r="D44" s="30"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A45" s="43"/>
-      <c r="B45" s="40"/>
-      <c r="C45" s="40"/>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="39"/>
+      <c r="B45" s="41"/>
+      <c r="C45" s="41"/>
       <c r="D45" s="30"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A46" s="43"/>
-      <c r="B46" s="40"/>
-      <c r="C46" s="40"/>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="39"/>
+      <c r="B46" s="41"/>
+      <c r="C46" s="41"/>
       <c r="D46" s="30"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A47" s="43"/>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="39"/>
       <c r="B47" s="24" t="s">
         <v>6</v>
       </c>
@@ -2000,46 +2018,46 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="44"/>
-      <c r="B48" s="37"/>
-      <c r="C48" s="37"/>
-      <c r="D48" s="38"/>
-    </row>
-    <row r="49" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A49" s="42">
+    <row r="48" spans="1:4" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="40"/>
+      <c r="B48" s="42"/>
+      <c r="C48" s="42"/>
+      <c r="D48" s="43"/>
+    </row>
+    <row r="49" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="38">
         <v>45441</v>
       </c>
-      <c r="B49" s="41"/>
-      <c r="C49" s="41"/>
+      <c r="B49" s="46"/>
+      <c r="C49" s="46"/>
       <c r="D49" s="36"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A50" s="43"/>
-      <c r="B50" s="40"/>
-      <c r="C50" s="40"/>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="39"/>
+      <c r="B50" s="41"/>
+      <c r="C50" s="41"/>
       <c r="D50" s="30"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A51" s="43"/>
-      <c r="B51" s="40"/>
-      <c r="C51" s="40"/>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" s="39"/>
+      <c r="B51" s="41"/>
+      <c r="C51" s="41"/>
       <c r="D51" s="30"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A52" s="43"/>
-      <c r="B52" s="40"/>
-      <c r="C52" s="40"/>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" s="39"/>
+      <c r="B52" s="41"/>
+      <c r="C52" s="41"/>
       <c r="D52" s="30"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A53" s="43"/>
-      <c r="B53" s="40"/>
-      <c r="C53" s="40"/>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="39"/>
+      <c r="B53" s="41"/>
+      <c r="C53" s="41"/>
       <c r="D53" s="30"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A54" s="43"/>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="39"/>
       <c r="B54" s="24" t="s">
         <v>6</v>
       </c>
@@ -2051,46 +2069,46 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="44"/>
-      <c r="B55" s="37"/>
-      <c r="C55" s="37"/>
-      <c r="D55" s="38"/>
-    </row>
-    <row r="56" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A56" s="42">
+    <row r="55" spans="1:4" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="40"/>
+      <c r="B55" s="42"/>
+      <c r="C55" s="42"/>
+      <c r="D55" s="43"/>
+    </row>
+    <row r="56" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="38">
         <v>45442</v>
       </c>
-      <c r="B56" s="41"/>
-      <c r="C56" s="41"/>
+      <c r="B56" s="46"/>
+      <c r="C56" s="46"/>
       <c r="D56" s="36"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A57" s="43"/>
-      <c r="B57" s="40"/>
-      <c r="C57" s="40"/>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" s="39"/>
+      <c r="B57" s="41"/>
+      <c r="C57" s="41"/>
       <c r="D57" s="30"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A58" s="43"/>
-      <c r="B58" s="40"/>
-      <c r="C58" s="40"/>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" s="39"/>
+      <c r="B58" s="41"/>
+      <c r="C58" s="41"/>
       <c r="D58" s="30"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A59" s="43"/>
-      <c r="B59" s="40"/>
-      <c r="C59" s="40"/>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" s="39"/>
+      <c r="B59" s="41"/>
+      <c r="C59" s="41"/>
       <c r="D59" s="30"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A60" s="43"/>
-      <c r="B60" s="40"/>
-      <c r="C60" s="40"/>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" s="39"/>
+      <c r="B60" s="41"/>
+      <c r="C60" s="41"/>
       <c r="D60" s="30"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A61" s="43"/>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" s="39"/>
       <c r="B61" s="24" t="s">
         <v>6</v>
       </c>
@@ -2102,44 +2120,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="44"/>
-      <c r="B62" s="37"/>
-      <c r="C62" s="37"/>
-      <c r="D62" s="38"/>
-    </row>
-    <row r="63" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A63" s="42"/>
-      <c r="B63" s="41"/>
-      <c r="C63" s="41"/>
+    <row r="62" spans="1:4" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="40"/>
+      <c r="B62" s="42"/>
+      <c r="C62" s="42"/>
+      <c r="D62" s="43"/>
+    </row>
+    <row r="63" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="38"/>
+      <c r="B63" s="46"/>
+      <c r="C63" s="46"/>
       <c r="D63" s="36"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A64" s="43"/>
-      <c r="B64" s="40"/>
-      <c r="C64" s="40"/>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" s="39"/>
+      <c r="B64" s="41"/>
+      <c r="C64" s="41"/>
       <c r="D64" s="30"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A65" s="43"/>
-      <c r="B65" s="40"/>
-      <c r="C65" s="40"/>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" s="39"/>
+      <c r="B65" s="41"/>
+      <c r="C65" s="41"/>
       <c r="D65" s="30"/>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A66" s="43"/>
-      <c r="B66" s="40"/>
-      <c r="C66" s="40"/>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" s="39"/>
+      <c r="B66" s="41"/>
+      <c r="C66" s="41"/>
       <c r="D66" s="30"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A67" s="43"/>
-      <c r="B67" s="40"/>
-      <c r="C67" s="40"/>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" s="39"/>
+      <c r="B67" s="41"/>
+      <c r="C67" s="41"/>
       <c r="D67" s="30"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A68" s="43"/>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" s="39"/>
       <c r="B68" s="24" t="s">
         <v>6</v>
       </c>
@@ -2151,44 +2169,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="44"/>
-      <c r="B69" s="37"/>
-      <c r="C69" s="37"/>
-      <c r="D69" s="38"/>
-    </row>
-    <row r="70" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A70" s="42"/>
-      <c r="B70" s="41"/>
-      <c r="C70" s="41"/>
+    <row r="69" spans="1:4" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="40"/>
+      <c r="B69" s="42"/>
+      <c r="C69" s="42"/>
+      <c r="D69" s="43"/>
+    </row>
+    <row r="70" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="38"/>
+      <c r="B70" s="46"/>
+      <c r="C70" s="46"/>
       <c r="D70" s="36"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A71" s="43"/>
-      <c r="B71" s="40"/>
-      <c r="C71" s="40"/>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" s="39"/>
+      <c r="B71" s="41"/>
+      <c r="C71" s="41"/>
       <c r="D71" s="30"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A72" s="43"/>
-      <c r="B72" s="40"/>
-      <c r="C72" s="40"/>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" s="39"/>
+      <c r="B72" s="41"/>
+      <c r="C72" s="41"/>
       <c r="D72" s="30"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A73" s="43"/>
-      <c r="B73" s="40"/>
-      <c r="C73" s="40"/>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73" s="39"/>
+      <c r="B73" s="41"/>
+      <c r="C73" s="41"/>
       <c r="D73" s="30"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A74" s="43"/>
-      <c r="B74" s="40"/>
-      <c r="C74" s="40"/>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74" s="39"/>
+      <c r="B74" s="41"/>
+      <c r="C74" s="41"/>
       <c r="D74" s="30"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A75" s="43"/>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75" s="39"/>
       <c r="B75" s="24" t="s">
         <v>6</v>
       </c>
@@ -2200,44 +2218,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="44"/>
-      <c r="B76" s="37"/>
-      <c r="C76" s="37"/>
-      <c r="D76" s="38"/>
-    </row>
-    <row r="77" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A77" s="42"/>
-      <c r="B77" s="41"/>
-      <c r="C77" s="41"/>
+    <row r="76" spans="1:4" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="40"/>
+      <c r="B76" s="42"/>
+      <c r="C76" s="42"/>
+      <c r="D76" s="43"/>
+    </row>
+    <row r="77" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="38"/>
+      <c r="B77" s="46"/>
+      <c r="C77" s="46"/>
       <c r="D77" s="36"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A78" s="43"/>
-      <c r="B78" s="40"/>
-      <c r="C78" s="40"/>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78" s="39"/>
+      <c r="B78" s="41"/>
+      <c r="C78" s="41"/>
       <c r="D78" s="30"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A79" s="43"/>
-      <c r="B79" s="40"/>
-      <c r="C79" s="40"/>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A79" s="39"/>
+      <c r="B79" s="41"/>
+      <c r="C79" s="41"/>
       <c r="D79" s="30"/>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A80" s="43"/>
-      <c r="B80" s="40"/>
-      <c r="C80" s="40"/>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80" s="39"/>
+      <c r="B80" s="41"/>
+      <c r="C80" s="41"/>
       <c r="D80" s="30"/>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A81" s="43"/>
-      <c r="B81" s="40"/>
-      <c r="C81" s="40"/>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A81" s="39"/>
+      <c r="B81" s="41"/>
+      <c r="C81" s="41"/>
       <c r="D81" s="30"/>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A82" s="43"/>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A82" s="39"/>
       <c r="B82" s="24" t="s">
         <v>6</v>
       </c>
@@ -2249,13 +2267,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="44"/>
-      <c r="B83" s="45"/>
-      <c r="C83" s="45"/>
-      <c r="D83" s="46"/>
-    </row>
-    <row r="84" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:4" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="40"/>
+      <c r="B83" s="62"/>
+      <c r="C83" s="62"/>
+      <c r="D83" s="63"/>
+    </row>
+    <row r="84" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="33"/>
       <c r="B84" s="2"/>
       <c r="C84" s="18" t="s">
@@ -2263,19 +2281,80 @@
       </c>
       <c r="D84" s="27">
         <f>D13+D22+D28+D33+D40+D47+D54+D61+D68+D75+D82</f>
-        <v>30.5</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A85" s="62" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A85" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B85" s="62"/>
-      <c r="C85" s="62"/>
-      <c r="D85" s="62"/>
+      <c r="B85" s="37"/>
+      <c r="C85" s="37"/>
+      <c r="D85" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="77">
+    <mergeCell ref="B48:D48"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B55:D55"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="A77:A83"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="B78:C78"/>
+    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="B83:D83"/>
+    <mergeCell ref="A56:A62"/>
+    <mergeCell ref="A63:A69"/>
+    <mergeCell ref="B62:D62"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="A70:A76"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B76:D76"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="A6:A14"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="A24:A29"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="B4:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A4:A5"/>
     <mergeCell ref="A85:D85"/>
     <mergeCell ref="A15:A23"/>
     <mergeCell ref="B17:C17"/>
@@ -2292,74 +2371,13 @@
     <mergeCell ref="A42:A48"/>
     <mergeCell ref="B42:C42"/>
     <mergeCell ref="B43:C43"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="B4:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="A24:A29"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="A6:A14"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="A70:A76"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B76:D76"/>
-    <mergeCell ref="A56:A62"/>
-    <mergeCell ref="A63:A69"/>
-    <mergeCell ref="B62:D62"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B69:D69"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="A77:A83"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="B78:C78"/>
-    <mergeCell ref="B79:C79"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B81:C81"/>
-    <mergeCell ref="B83:D83"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B55:D55"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B48:D48"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
   </mergeCells>
   <conditionalFormatting sqref="D6:D13 D15:D22 D24:D28 D30:D33">
-    <cfRule type="containsText" dxfId="17" priority="24" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="17" priority="23" operator="containsText" text="Terminé">
+      <formula>NOT(ISERROR(SEARCH("Terminé",D6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="16" priority="24" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",D6)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="23" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",D6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35:D40">
@@ -2371,27 +2389,27 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D42:D47">
-    <cfRule type="containsText" dxfId="13" priority="10" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="13" priority="9" operator="containsText" text="Terminé">
+      <formula>NOT(ISERROR(SEARCH("Terminé",D42)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="10" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",D42)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="9" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",D42)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D49:D54">
-    <cfRule type="containsText" dxfId="11" priority="8" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="11" priority="7" operator="containsText" text="Terminé">
+      <formula>NOT(ISERROR(SEARCH("Terminé",D49)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="8" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",D49)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="7" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",D49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D56:D61">
-    <cfRule type="containsText" dxfId="9" priority="6" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="9" priority="5" operator="containsText" text="Terminé">
+      <formula>NOT(ISERROR(SEARCH("Terminé",D56)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="6" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",D56)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="5" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",D56)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D63:D68">
@@ -2411,19 +2429,19 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D77:D82">
-    <cfRule type="containsText" dxfId="3" priority="12" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="3" priority="11" operator="containsText" text="Terminé">
+      <formula>NOT(ISERROR(SEARCH("Terminé",D77)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="12" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",D77)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="11" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",D77)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D84">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Terminé">
+      <formula>NOT(ISERROR(SEARCH("Terminé",D84)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",D84)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",D84)))</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions horizontalCentered="1"/>

</xml_diff>

<commit_message>
Add popups and better exception handling
</commit_message>
<xml_diff>
--- a/docs/3_CAND_Modele_Journal_2024.xlsx
+++ b/docs/3_CAND_Modele_Journal_2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\tests\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F85AD907-90FB-46A5-BC95-F713593D914B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B49772EA-0C5F-48E4-BEE3-9B81AB84BC2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-165" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal" sheetId="8" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Journal!$A$5:$HI$5</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Journal!$B:$D,Journal!$1:$5</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Journal!$A$1:$D$83</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Journal!$A$1:$D$84</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="54">
   <si>
     <t>Insérer les lignes au-dessus de celle-ci !</t>
   </si>
@@ -221,6 +221,32 @@
   <si>
     <t>J'ai assez bien avancé sur l'analyse. Je sens que les diagrammes ne seront pas un gros problème pour ce projet et ça me donne confiance!
 J'ai eus un rdv avec Erasmus</t>
+  </si>
+  <si>
+    <t>Deuxième visite des experts</t>
+  </si>
+  <si>
+    <t>Modification de certains diagrammes, encorager à utiiser les mêmes noms dans tous les diagrammes, regrouper les feux de signalisation pour la version du TPI, modification de la date de la présenation (14/06 10h15 A32), informations à propos du WebSumarry et demande d'envoyer le planning et le journal ce vendredi midi</t>
+  </si>
+  <si>
+    <t>Gestion de la création de compte</t>
+  </si>
+  <si>
+    <t>Gestion de la connection à un compte</t>
+  </si>
+  <si>
+    <t>/ La réfléction personnelle de cette journée à été réalisé le 28.05.2024 /
+Journée plutôt satifaisante, un bon nombre de diagrammes ont été réalisé aujourd'hui</t>
+  </si>
+  <si>
+    <t>/ La réfléction personnelle de cette journée à été réalisé le 28.05.2024 /
+La première partie de l'implémentation m'a pris plus de temps que prévu, additionellement j'ai eus le problème avec NetBeans et je suis assez frustré. Mis à part cela, tous se passe relativement bien!</t>
+  </si>
+  <si>
+    <t>Aujourd'hui était une bonne journée de développement mais j'ai senti que je travaillais beaucoup plus lentement sans musique. Je penserai à prendre mes écouteurs demain !</t>
+  </si>
+  <si>
+    <t>Gestion des pop-up</t>
   </si>
 </sst>
 </file>
@@ -734,7 +760,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -876,112 +902,116 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1555,12 +1585,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H84"/>
+  <dimension ref="A1:H85"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft"/>
       <selection activeCell="D5" sqref="A5:XFD5"/>
-      <selection pane="bottomLeft" activeCell="I36" sqref="I36"/>
+      <selection pane="bottomLeft" activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1573,19 +1603,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
     </row>
     <row r="2" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="57"/>
-      <c r="C2" s="58"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="62"/>
       <c r="D2" s="21">
         <v>148477</v>
       </c>
@@ -1598,13 +1628,13 @@
       <c r="H3" s="8"/>
     </row>
     <row r="4" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="59" t="s">
+      <c r="A4" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="52" t="s">
+      <c r="B4" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="53"/>
+      <c r="C4" s="57"/>
       <c r="D4" s="28" t="s">
         <v>4</v>
       </c>
@@ -1615,9 +1645,9 @@
       <c r="H4" s="10"/>
     </row>
     <row r="5" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="60"/>
-      <c r="B5" s="54"/>
-      <c r="C5" s="55"/>
+      <c r="A5" s="64"/>
+      <c r="B5" s="58"/>
+      <c r="C5" s="59"/>
       <c r="D5" s="29" t="s">
         <v>3</v>
       </c>
@@ -1628,13 +1658,13 @@
       <c r="H5" s="12"/>
     </row>
     <row r="6" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="41">
+      <c r="A6" s="46">
         <v>45433</v>
       </c>
-      <c r="B6" s="56" t="s">
+      <c r="B6" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="56"/>
+      <c r="C6" s="60"/>
       <c r="D6" s="31">
         <v>1.5</v>
       </c>
@@ -1645,11 +1675,11 @@
       <c r="H6" s="14"/>
     </row>
     <row r="7" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="42"/>
-      <c r="B7" s="63" t="s">
+      <c r="A7" s="47"/>
+      <c r="B7" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="63"/>
+      <c r="C7" s="51"/>
       <c r="D7" s="32">
         <v>1</v>
       </c>
@@ -1660,7 +1690,7 @@
       <c r="H7" s="17"/>
     </row>
     <row r="8" spans="1:8" ht="56.25" x14ac:dyDescent="0.2">
-      <c r="A8" s="42"/>
+      <c r="A8" s="47"/>
       <c r="B8" s="19" t="s">
         <v>25</v>
       </c>
@@ -1672,25 +1702,25 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="42"/>
-      <c r="B9" s="48"/>
-      <c r="C9" s="48"/>
+      <c r="A9" s="47"/>
+      <c r="B9" s="43"/>
+      <c r="C9" s="43"/>
       <c r="D9" s="30">
         <v>1.5</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="42"/>
-      <c r="B10" s="48" t="s">
+      <c r="A10" s="47"/>
+      <c r="B10" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="48"/>
+      <c r="C10" s="43"/>
       <c r="D10" s="30">
         <v>0.5</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="42"/>
+      <c r="A11" s="47"/>
       <c r="B11" s="22" t="s">
         <v>19</v>
       </c>
@@ -1702,7 +1732,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="42"/>
+      <c r="A12" s="47"/>
       <c r="B12" s="24" t="s">
         <v>6</v>
       </c>
@@ -1715,15 +1745,15 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="43"/>
-      <c r="B13" s="45" t="s">
+      <c r="A13" s="48"/>
+      <c r="B13" s="41" t="s">
         <v>45</v>
       </c>
-      <c r="C13" s="45"/>
-      <c r="D13" s="46"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="42"/>
     </row>
     <row r="14" spans="1:8" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A14" s="41">
+      <c r="A14" s="46">
         <v>45434</v>
       </c>
       <c r="B14" s="34" t="s">
@@ -1737,17 +1767,17 @@
       </c>
     </row>
     <row r="15" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="42"/>
-      <c r="B15" s="50" t="s">
+      <c r="A15" s="47"/>
+      <c r="B15" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="50"/>
+      <c r="C15" s="52"/>
       <c r="D15" s="30">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="42"/>
+      <c r="A16" s="47"/>
       <c r="B16" s="44" t="s">
         <v>14</v>
       </c>
@@ -1757,7 +1787,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="67.5" x14ac:dyDescent="0.2">
-      <c r="A17" s="42"/>
+      <c r="A17" s="47"/>
       <c r="B17" s="19" t="s">
         <v>13</v>
       </c>
@@ -1769,7 +1799,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="45" x14ac:dyDescent="0.2">
-      <c r="A18" s="42"/>
+      <c r="A18" s="47"/>
       <c r="B18" s="19" t="s">
         <v>25</v>
       </c>
@@ -1781,27 +1811,27 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="42"/>
-      <c r="B19" s="48" t="s">
+      <c r="A19" s="47"/>
+      <c r="B19" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="48"/>
+      <c r="C19" s="43"/>
       <c r="D19" s="30">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="42"/>
-      <c r="B20" s="61" t="s">
+      <c r="A20" s="47"/>
+      <c r="B20" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="62"/>
+      <c r="C20" s="54"/>
       <c r="D20" s="30">
         <v>3.5</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="42"/>
+      <c r="A21" s="47"/>
       <c r="B21" s="24" t="s">
         <v>6</v>
       </c>
@@ -1814,55 +1844,55 @@
       </c>
     </row>
     <row r="22" spans="1:4" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="43"/>
-      <c r="B22" s="45" t="s">
+      <c r="A22" s="48"/>
+      <c r="B22" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="45"/>
-      <c r="D22" s="46"/>
+      <c r="C22" s="41"/>
+      <c r="D22" s="42"/>
     </row>
     <row r="23" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="41">
+      <c r="A23" s="46">
         <v>45435</v>
       </c>
-      <c r="B23" s="50" t="s">
+      <c r="B23" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="50"/>
+      <c r="C23" s="52"/>
       <c r="D23" s="36"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="42"/>
-      <c r="B24" s="61" t="s">
+      <c r="A24" s="47"/>
+      <c r="B24" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="C24" s="62"/>
+      <c r="C24" s="54"/>
       <c r="D24" s="30">
         <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="42"/>
-      <c r="B25" s="48" t="s">
+      <c r="A25" s="47"/>
+      <c r="B25" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="48"/>
+      <c r="C25" s="43"/>
       <c r="D25" s="30">
         <v>2.5</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="42"/>
-      <c r="B26" s="48" t="s">
+      <c r="A26" s="47"/>
+      <c r="B26" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="C26" s="48"/>
+      <c r="C26" s="43"/>
       <c r="D26" s="30">
         <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="42"/>
+      <c r="A27" s="47"/>
       <c r="B27" s="24" t="s">
         <v>6</v>
       </c>
@@ -1875,25 +1905,27 @@
       </c>
     </row>
     <row r="28" spans="1:4" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="43"/>
-      <c r="B28" s="45"/>
-      <c r="C28" s="45"/>
-      <c r="D28" s="46"/>
+      <c r="A28" s="48"/>
+      <c r="B28" s="41" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28" s="41"/>
+      <c r="D28" s="42"/>
     </row>
     <row r="29" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="41">
+      <c r="A29" s="46">
         <v>45436</v>
       </c>
-      <c r="B29" s="47" t="s">
+      <c r="B29" s="66" t="s">
         <v>10</v>
       </c>
-      <c r="C29" s="47"/>
+      <c r="C29" s="66"/>
       <c r="D29" s="36">
         <v>4.5</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="56.25" x14ac:dyDescent="0.2">
-      <c r="A30" s="42"/>
+      <c r="A30" s="47"/>
       <c r="B30" s="19" t="s">
         <v>25</v>
       </c>
@@ -1905,17 +1937,17 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="42"/>
-      <c r="B31" s="48" t="s">
+      <c r="A31" s="47"/>
+      <c r="B31" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="C31" s="48"/>
+      <c r="C31" s="43"/>
       <c r="D31" s="30">
         <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="42"/>
+      <c r="A32" s="47"/>
       <c r="B32" s="24" t="s">
         <v>6</v>
       </c>
@@ -1928,37 +1960,37 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="43"/>
-      <c r="B33" s="45" t="s">
+      <c r="A33" s="48"/>
+      <c r="B33" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="C33" s="45"/>
-      <c r="D33" s="46"/>
+      <c r="C33" s="41"/>
+      <c r="D33" s="42"/>
     </row>
     <row r="34" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="41">
+      <c r="A34" s="46">
         <v>45439</v>
       </c>
-      <c r="B34" s="49" t="s">
+      <c r="B34" s="67" t="s">
         <v>35</v>
       </c>
-      <c r="C34" s="49"/>
+      <c r="C34" s="67"/>
       <c r="D34" s="36">
         <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="42"/>
-      <c r="B35" s="48" t="s">
+      <c r="A35" s="47"/>
+      <c r="B35" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="C35" s="48"/>
+      <c r="C35" s="43"/>
       <c r="D35" s="30">
         <v>2.5</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A36" s="42"/>
+      <c r="A36" s="47"/>
       <c r="B36" s="37" t="s">
         <v>37</v>
       </c>
@@ -1970,17 +2002,17 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="42"/>
-      <c r="B37" s="48" t="s">
+      <c r="A37" s="47"/>
+      <c r="B37" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="C37" s="48"/>
+      <c r="C37" s="43"/>
       <c r="D37" s="30">
         <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="45" x14ac:dyDescent="0.2">
-      <c r="A38" s="42"/>
+      <c r="A38" s="47"/>
       <c r="B38" s="22" t="s">
         <v>42</v>
       </c>
@@ -1992,7 +2024,7 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="42"/>
+      <c r="A39" s="47"/>
       <c r="B39" s="24" t="s">
         <v>6</v>
       </c>
@@ -2004,14 +2036,16 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="43"/>
-      <c r="B40" s="45"/>
-      <c r="C40" s="45"/>
-      <c r="D40" s="46"/>
+    <row r="40" spans="1:4" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="48"/>
+      <c r="B40" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="C40" s="41"/>
+      <c r="D40" s="42"/>
     </row>
     <row r="41" spans="1:4" ht="56.25" x14ac:dyDescent="0.2">
-      <c r="A41" s="41">
+      <c r="A41" s="46">
         <v>45440</v>
       </c>
       <c r="B41" s="34" t="s">
@@ -2025,378 +2059,349 @@
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="42"/>
-      <c r="B42" s="48" t="s">
+      <c r="A42" s="47"/>
+      <c r="B42" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="C42" s="48"/>
-      <c r="D42" s="30"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="42"/>
-      <c r="B43" s="44"/>
-      <c r="C43" s="44"/>
-      <c r="D43" s="30"/>
+      <c r="C42" s="43"/>
+      <c r="D42" s="30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="90" x14ac:dyDescent="0.2">
+      <c r="A43" s="47"/>
+      <c r="B43" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C43" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="D43" s="30">
+        <v>1</v>
+      </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="42"/>
-      <c r="B44" s="44"/>
-      <c r="C44" s="44"/>
-      <c r="D44" s="30"/>
+      <c r="A44" s="47"/>
+      <c r="B44" s="43" t="s">
+        <v>48</v>
+      </c>
+      <c r="C44" s="43"/>
+      <c r="D44" s="30">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="42"/>
-      <c r="B45" s="44"/>
-      <c r="C45" s="44"/>
-      <c r="D45" s="30"/>
+      <c r="A45" s="47"/>
+      <c r="B45" s="43" t="s">
+        <v>49</v>
+      </c>
+      <c r="C45" s="43"/>
+      <c r="D45" s="30">
+        <v>1</v>
+      </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="42"/>
-      <c r="B46" s="24" t="s">
+      <c r="A46" s="47"/>
+      <c r="B46" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="C46" s="40"/>
+      <c r="D46" s="30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="47"/>
+      <c r="B47" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="C46" s="25" t="s">
+      <c r="C47" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="D46" s="30">
-        <f>SUM(D41:D45)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="43"/>
-      <c r="B47" s="45"/>
-      <c r="C47" s="45"/>
-      <c r="D47" s="46"/>
-    </row>
-    <row r="48" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="41">
+      <c r="D47" s="30">
+        <f>SUM(D41:D46)</f>
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="48"/>
+      <c r="B48" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="C48" s="41"/>
+      <c r="D48" s="42"/>
+    </row>
+    <row r="49" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="46">
         <v>45441</v>
       </c>
-      <c r="B48" s="64"/>
-      <c r="C48" s="64"/>
-      <c r="D48" s="36"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="42"/>
-      <c r="B49" s="44"/>
-      <c r="C49" s="44"/>
-      <c r="D49" s="30"/>
+      <c r="B49" s="45"/>
+      <c r="C49" s="45"/>
+      <c r="D49" s="36"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" s="42"/>
+      <c r="A50" s="47"/>
       <c r="B50" s="44"/>
       <c r="C50" s="44"/>
       <c r="D50" s="30"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" s="42"/>
+      <c r="A51" s="47"/>
       <c r="B51" s="44"/>
       <c r="C51" s="44"/>
       <c r="D51" s="30"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" s="42"/>
+      <c r="A52" s="47"/>
       <c r="B52" s="44"/>
       <c r="C52" s="44"/>
       <c r="D52" s="30"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" s="42"/>
-      <c r="B53" s="24" t="s">
+      <c r="A53" s="47"/>
+      <c r="B53" s="44"/>
+      <c r="C53" s="44"/>
+      <c r="D53" s="30"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="47"/>
+      <c r="B54" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="C53" s="25" t="s">
+      <c r="C54" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="D53" s="30">
-        <f>SUM(D48:D52)</f>
+      <c r="D54" s="30">
+        <f>SUM(D49:D53)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="43"/>
-      <c r="B54" s="45"/>
-      <c r="C54" s="45"/>
-      <c r="D54" s="46"/>
-    </row>
-    <row r="55" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="41">
+    <row r="55" spans="1:4" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="48"/>
+      <c r="B55" s="41"/>
+      <c r="C55" s="41"/>
+      <c r="D55" s="42"/>
+    </row>
+    <row r="56" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="46">
         <v>45442</v>
       </c>
-      <c r="B55" s="64"/>
-      <c r="C55" s="64"/>
-      <c r="D55" s="36"/>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" s="42"/>
-      <c r="B56" s="44"/>
-      <c r="C56" s="44"/>
-      <c r="D56" s="30"/>
+      <c r="B56" s="45"/>
+      <c r="C56" s="45"/>
+      <c r="D56" s="36"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" s="42"/>
+      <c r="A57" s="47"/>
       <c r="B57" s="44"/>
       <c r="C57" s="44"/>
       <c r="D57" s="30"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" s="42"/>
+      <c r="A58" s="47"/>
       <c r="B58" s="44"/>
       <c r="C58" s="44"/>
       <c r="D58" s="30"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" s="42"/>
+      <c r="A59" s="47"/>
       <c r="B59" s="44"/>
       <c r="C59" s="44"/>
       <c r="D59" s="30"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" s="42"/>
-      <c r="B60" s="24" t="s">
+      <c r="A60" s="47"/>
+      <c r="B60" s="44"/>
+      <c r="C60" s="44"/>
+      <c r="D60" s="30"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" s="47"/>
+      <c r="B61" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="C60" s="25" t="s">
+      <c r="C61" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="D60" s="30">
-        <f>SUM(D55:D59)</f>
+      <c r="D61" s="30">
+        <f>SUM(D56:D60)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="43"/>
-      <c r="B61" s="45"/>
-      <c r="C61" s="45"/>
-      <c r="D61" s="46"/>
-    </row>
-    <row r="62" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="41"/>
-      <c r="B62" s="64"/>
-      <c r="C62" s="64"/>
-      <c r="D62" s="36"/>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" s="42"/>
-      <c r="B63" s="44"/>
-      <c r="C63" s="44"/>
-      <c r="D63" s="30"/>
+    <row r="62" spans="1:4" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="48"/>
+      <c r="B62" s="41"/>
+      <c r="C62" s="41"/>
+      <c r="D62" s="42"/>
+    </row>
+    <row r="63" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="46"/>
+      <c r="B63" s="45"/>
+      <c r="C63" s="45"/>
+      <c r="D63" s="36"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" s="42"/>
+      <c r="A64" s="47"/>
       <c r="B64" s="44"/>
       <c r="C64" s="44"/>
       <c r="D64" s="30"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" s="42"/>
+      <c r="A65" s="47"/>
       <c r="B65" s="44"/>
       <c r="C65" s="44"/>
       <c r="D65" s="30"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" s="42"/>
+      <c r="A66" s="47"/>
       <c r="B66" s="44"/>
       <c r="C66" s="44"/>
       <c r="D66" s="30"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" s="42"/>
-      <c r="B67" s="24" t="s">
+      <c r="A67" s="47"/>
+      <c r="B67" s="44"/>
+      <c r="C67" s="44"/>
+      <c r="D67" s="30"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" s="47"/>
+      <c r="B68" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="C67" s="25" t="s">
+      <c r="C68" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="D67" s="30">
-        <f>SUM(D62:D66)</f>
+      <c r="D68" s="30">
+        <f>SUM(D63:D67)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="43"/>
-      <c r="B68" s="45"/>
-      <c r="C68" s="45"/>
-      <c r="D68" s="46"/>
-    </row>
-    <row r="69" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="41"/>
-      <c r="B69" s="64"/>
-      <c r="C69" s="64"/>
-      <c r="D69" s="36"/>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" s="42"/>
-      <c r="B70" s="44"/>
-      <c r="C70" s="44"/>
-      <c r="D70" s="30"/>
+    <row r="69" spans="1:4" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="48"/>
+      <c r="B69" s="41"/>
+      <c r="C69" s="41"/>
+      <c r="D69" s="42"/>
+    </row>
+    <row r="70" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="46"/>
+      <c r="B70" s="45"/>
+      <c r="C70" s="45"/>
+      <c r="D70" s="36"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" s="42"/>
+      <c r="A71" s="47"/>
       <c r="B71" s="44"/>
       <c r="C71" s="44"/>
       <c r="D71" s="30"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" s="42"/>
+      <c r="A72" s="47"/>
       <c r="B72" s="44"/>
       <c r="C72" s="44"/>
       <c r="D72" s="30"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" s="42"/>
+      <c r="A73" s="47"/>
       <c r="B73" s="44"/>
       <c r="C73" s="44"/>
       <c r="D73" s="30"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" s="42"/>
-      <c r="B74" s="24" t="s">
+      <c r="A74" s="47"/>
+      <c r="B74" s="44"/>
+      <c r="C74" s="44"/>
+      <c r="D74" s="30"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75" s="47"/>
+      <c r="B75" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="C74" s="25" t="s">
+      <c r="C75" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="D74" s="30">
-        <f>SUM(D69:D73)</f>
+      <c r="D75" s="30">
+        <f>SUM(D70:D74)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="43"/>
-      <c r="B75" s="45"/>
-      <c r="C75" s="45"/>
-      <c r="D75" s="46"/>
-    </row>
-    <row r="76" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="41"/>
-      <c r="B76" s="64"/>
-      <c r="C76" s="64"/>
-      <c r="D76" s="36"/>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A77" s="42"/>
-      <c r="B77" s="44"/>
-      <c r="C77" s="44"/>
-      <c r="D77" s="30"/>
+    <row r="76" spans="1:4" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="48"/>
+      <c r="B76" s="41"/>
+      <c r="C76" s="41"/>
+      <c r="D76" s="42"/>
+    </row>
+    <row r="77" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="46"/>
+      <c r="B77" s="45"/>
+      <c r="C77" s="45"/>
+      <c r="D77" s="36"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A78" s="42"/>
+      <c r="A78" s="47"/>
       <c r="B78" s="44"/>
       <c r="C78" s="44"/>
       <c r="D78" s="30"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79" s="42"/>
+      <c r="A79" s="47"/>
       <c r="B79" s="44"/>
       <c r="C79" s="44"/>
       <c r="D79" s="30"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80" s="42"/>
+      <c r="A80" s="47"/>
       <c r="B80" s="44"/>
       <c r="C80" s="44"/>
       <c r="D80" s="30"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A81" s="42"/>
-      <c r="B81" s="24" t="s">
+      <c r="A81" s="47"/>
+      <c r="B81" s="44"/>
+      <c r="C81" s="44"/>
+      <c r="D81" s="30"/>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A82" s="47"/>
+      <c r="B82" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="C81" s="25" t="s">
+      <c r="C82" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="D81" s="30">
-        <f>SUM(D76:D80)</f>
+      <c r="D82" s="30">
+        <f>SUM(D77:D81)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="43"/>
-      <c r="B82" s="65"/>
-      <c r="C82" s="65"/>
-      <c r="D82" s="66"/>
-    </row>
-    <row r="83" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="33"/>
-      <c r="B83" s="2"/>
-      <c r="C83" s="18" t="s">
+    <row r="83" spans="1:4" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="48"/>
+      <c r="B83" s="49"/>
+      <c r="C83" s="49"/>
+      <c r="D83" s="50"/>
+    </row>
+    <row r="84" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="33"/>
+      <c r="B84" s="2"/>
+      <c r="C84" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="D83" s="27">
-        <f>D12+D21+D27+D32+D39+D46+D53+D60+D67+D74+D81</f>
-        <v>38</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A84" s="40" t="s">
+      <c r="D84" s="27">
+        <f>D12+D21+D27+D32+D39+D47+D54+D61+D68+D75+D82</f>
+        <v>45.5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A85" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="B84" s="40"/>
-      <c r="C84" s="40"/>
-      <c r="D84" s="40"/>
+      <c r="B85" s="65"/>
+      <c r="C85" s="65"/>
+      <c r="D85" s="65"/>
     </row>
   </sheetData>
-  <mergeCells count="73">
-    <mergeCell ref="B47:D47"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="A76:A82"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="B78:C78"/>
-    <mergeCell ref="B79:C79"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B82:D82"/>
-    <mergeCell ref="A55:A61"/>
-    <mergeCell ref="A62:A68"/>
-    <mergeCell ref="B61:D61"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B68:D68"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="A69:A75"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B75:D75"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="A6:A13"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="A23:A28"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="B4:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A84:D84"/>
+  <mergeCells count="72">
+    <mergeCell ref="A85:D85"/>
     <mergeCell ref="A14:A22"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="B22:D22"/>
@@ -2407,13 +2412,69 @@
     <mergeCell ref="A34:A40"/>
     <mergeCell ref="B34:C34"/>
     <mergeCell ref="B35:C35"/>
-    <mergeCell ref="A48:A54"/>
-    <mergeCell ref="A41:A47"/>
+    <mergeCell ref="A49:A55"/>
+    <mergeCell ref="A41:A48"/>
     <mergeCell ref="B42:C42"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B20:C20"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="B4:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="A23:A28"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="A6:A13"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="A70:A76"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B76:D76"/>
+    <mergeCell ref="A56:A62"/>
+    <mergeCell ref="A63:A69"/>
+    <mergeCell ref="B62:D62"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="A77:A83"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="B78:C78"/>
+    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="B83:D83"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B55:D55"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B48:D48"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
   </mergeCells>
-  <conditionalFormatting sqref="D14:D21 D23:D27 D29:D32 D6:D12">
+  <conditionalFormatting sqref="D6:D12 D14:D21 D23:D27 D29:D32">
     <cfRule type="containsText" dxfId="17" priority="23" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",D6)))</formula>
     </cfRule>
@@ -2429,7 +2490,7 @@
       <formula>NOT(ISERROR(SEARCH("En cours",D34)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D41:D46">
+  <conditionalFormatting sqref="D41:D47">
     <cfRule type="containsText" dxfId="13" priority="9" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",D41)))</formula>
     </cfRule>
@@ -2437,52 +2498,52 @@
       <formula>NOT(ISERROR(SEARCH("En cours",D41)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D48:D53">
+  <conditionalFormatting sqref="D49:D54">
     <cfRule type="containsText" dxfId="11" priority="7" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",D48)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Terminé",D49)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="10" priority="8" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",D48)))</formula>
+      <formula>NOT(ISERROR(SEARCH("En cours",D49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D55:D60">
+  <conditionalFormatting sqref="D56:D61">
     <cfRule type="containsText" dxfId="9" priority="5" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",D55)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Terminé",D56)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="8" priority="6" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",D55)))</formula>
+      <formula>NOT(ISERROR(SEARCH("En cours",D56)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D62:D67">
+  <conditionalFormatting sqref="D63:D68">
     <cfRule type="containsText" dxfId="7" priority="15" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",D62)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Terminé",D63)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="6" priority="16" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",D62)))</formula>
+      <formula>NOT(ISERROR(SEARCH("En cours",D63)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D69:D74">
+  <conditionalFormatting sqref="D70:D75">
     <cfRule type="containsText" dxfId="5" priority="13" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",D69)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Terminé",D70)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="4" priority="14" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",D69)))</formula>
+      <formula>NOT(ISERROR(SEARCH("En cours",D70)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D76:D81">
+  <conditionalFormatting sqref="D77:D82">
     <cfRule type="containsText" dxfId="3" priority="11" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",D76)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Terminé",D77)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="2" priority="12" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",D76)))</formula>
+      <formula>NOT(ISERROR(SEARCH("En cours",D77)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D83">
+  <conditionalFormatting sqref="D84">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",D83)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Terminé",D84)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",D83)))</formula>
+      <formula>NOT(ISERROR(SEARCH("En cours",D84)))</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions horizontalCentered="1"/>
@@ -2494,8 +2555,8 @@
     <oddFooter>&amp;L&amp;8&amp;F&amp;R&amp;8Page &amp;P/&amp;N</oddFooter>
   </headerFooter>
   <rowBreaks count="2" manualBreakCount="2">
-    <brk id="47" max="16383" man="1"/>
-    <brk id="83" max="3" man="1"/>
+    <brk id="48" max="16383" man="1"/>
+    <brk id="84" max="3" man="1"/>
   </rowBreaks>
   <legacyDrawingHF r:id="rId2"/>
 </worksheet>

</xml_diff>